<commit_message>
Update timetracking and risk analysis
</commit_message>
<xml_diff>
--- a/Dokumentation/00_Projektplanung/Projektplan/TechnischeRisiken.xlsx
+++ b/Dokumentation/00_Projektplanung/Projektplan/TechnischeRisiken.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janik\OneDrive\Studium\Studienarbeit\SA-Git\Network-Unit-Testing\Dokumentation\00_Projektplanung\Projektplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-Stuff\Network-Unit-Testing\Dokumentation\00_Projektplanung\Projektplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{7B481570-66DF-411A-9154-E505172DC0B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{31E8590A-C6A0-49B7-98EE-C07E64AA4D9C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD0AEA6-1C79-4452-BE38-338962177743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Risikotabelle" sheetId="1" r:id="rId1"/>
+    <sheet name="Stand Analyse 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -228,6 +229,21 @@
   </si>
   <si>
     <t>Die als Ziel gesetzten Funktionen sind zu komplex und es müssen wesentliche Funktionalitäten weggelassen werden.</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>Requirements nicht verstanden</t>
+  </si>
+  <si>
+    <t>Die Arbeit entspricht nicht den vom Kunden gewünschten Anforderungen</t>
+  </si>
+  <si>
+    <t>Mittels Workshop und Requirements erfassung Risiko minimieren</t>
+  </si>
+  <si>
+    <t>Ist bereits eingetreten und hat 16 Stunden Aufwand gekostet</t>
   </si>
 </sst>
 </file>
@@ -265,12 +281,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -286,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,16 +361,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -364,7 +401,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -684,14 +721,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
@@ -702,63 +739,64 @@
     <col min="7" max="7" width="26" style="1" customWidth="1"/>
     <col min="8" max="8" width="26.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="30.140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="7.28515625" style="1"/>
+    <col min="10" max="10" width="43.140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="7.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="2">
         <f>SUM(F8:F16)</f>
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -787,7 +825,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
@@ -804,7 +842,7 @@
         <v>0.2</v>
       </c>
       <c r="F8" s="7">
-        <f t="shared" ref="F8:F15" si="0">D8*E8</f>
+        <f t="shared" ref="F8:F16" si="0">D8*E8</f>
         <v>8</v>
       </c>
       <c r="G8" s="7" t="s">
@@ -817,7 +855,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
@@ -847,7 +885,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
@@ -877,7 +915,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -907,7 +945,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
@@ -937,7 +975,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>21</v>
       </c>
@@ -967,7 +1005,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>26</v>
       </c>
@@ -997,7 +1035,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>27</v>
       </c>
@@ -1027,29 +1065,52 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+    <row r="16" spans="1:10" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="7">
+        <v>16</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="19"/>
       <c r="D17" s="12">
-        <f>SUM(D8:D15)</f>
-        <v>127</v>
+        <f>SUM(D8:D16)</f>
+        <v>143</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="12">
-        <f>SUM(F8:F15)</f>
-        <v>15.4</v>
+        <f>SUM(F8:F16)</f>
+        <v>23.4</v>
       </c>
     </row>
   </sheetData>
@@ -1065,4 +1126,387 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5BB8E9-85B9-40A0-BBB2-9EB8FC58D2A5}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="13" style="17" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="26" style="17" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="7.28515625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="18">
+        <f>SUM(F8:F16)</f>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="7">
+        <v>40</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" ref="F8:F15" si="0">D8*E8</f>
+        <v>8</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7">
+        <v>20</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="7">
+        <v>10</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="7">
+        <v>16</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="7">
+        <v>16</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="7">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="13">
+        <v>10</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="13">
+        <v>10</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="D17" s="16">
+        <f>SUM(D8:D15)</f>
+        <v>127</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="16">
+        <f>SUM(F8:F15)</f>
+        <v>15.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>